<commit_message>
all notebooks and shit
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/model_parameters/shocks/shocks.xlsx
+++ b/data/EPNM/interim/model_parameters/shocks/shocks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pichler" sheetId="1" state="visible" r:id="rId2"/>
@@ -330,11 +330,11 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1443,7 +1443,7 @@
       <selection pane="topLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -2552,7 +2552,7 @@
       <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -3661,7 +3661,7 @@
       <selection pane="topLeft" activeCell="J34" activeCellId="0" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -4770,7 +4770,7 @@
       <selection pane="topLeft" activeCell="J25" activeCellId="0" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.91"/>
@@ -5881,11 +5881,11 @@
   </sheetPr>
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.91"/>
@@ -7000,7 +7000,7 @@
       <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.91"/>
@@ -8115,7 +8115,7 @@
       <selection pane="topLeft" activeCell="M24" activeCellId="0" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.91"/>

</xml_diff>

<commit_message>
update parameters after sensitivity analysis
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/model_parameters/shocks/shocks.xlsx
+++ b/data/EPNM/interim/model_parameters/shocks/shocks.xlsx
@@ -325,7 +325,7 @@
       <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
@@ -1238,11 +1238,11 @@
   </sheetPr>
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B63" activeCellId="0" sqref="B63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.91"/>
@@ -1685,7 +1685,7 @@
         <v>33</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>-61.5</v>
@@ -1699,7 +1699,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="C33" s="1" t="n">
         <v>-61.5</v>
@@ -1713,7 +1713,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>-50</v>
+        <v>-30</v>
       </c>
       <c r="C34" s="1" t="n">
         <v>-45</v>

</xml_diff>